<commit_message>
Conexion a BD y correccion de cronograma
Se corrigio el cronograma a tiempo real de lo que se realizara y se agrego al documento la conexion de base de dato usando PHPMyAdmin para un proyecto desarrollado en Java utilizando NetBeans, etc.

Rafa
Moises
David
Ismael
Jorge
Kely
Jovani
Dduardo

Co-Authored-By: David Velázquez <steinervalue@users.noreply.github.com>
Co-Authored-By: ismaelmargarito <ismaelmargarito@users.noreply.github.com>
Co-Authored-By: moisesvidal <moisesvidal@users.noreply.github.com>
Co-Authored-By: ajovanny <ajovanny@users.noreply.github.com>
Co-Authored-By: Jorge Pérez Flores <jp1rish@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Cronograma y tiempo/Cronograma BD.xlsx
+++ b/Cronograma y tiempo/Cronograma BD.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2E10878-7C02-46BF-BDDA-A313F4E947D7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{305835F7-1252-49D9-A270-40BF02AB6CFD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1055,6 +1055,15 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1082,15 +1091,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="50">
@@ -1146,6 +1146,15 @@
     <cellStyle name="zHiddenText" xfId="3" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
   </cellStyles>
   <dxfs count="54">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1974,15 +1983,6 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <border>
         <left style="thin">
           <color theme="0" tint="-0.24994659260841701"/>
@@ -2303,9 +2303,9 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Descripción del hito" dataDxfId="41"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Categoría" dataDxfId="40"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Asignado a" dataDxfId="39"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Descripción del hito" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Categoría" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Asignado a" dataDxfId="0"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Progreso"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Inicio" dataCellStyle="Fecha"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Número de días"/>
@@ -2587,8 +2587,8 @@
   </sheetPr>
   <dimension ref="A1:BL40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2631,36 +2631,36 @@
       <c r="C2" s="15"/>
       <c r="F2" s="19"/>
       <c r="G2" s="17"/>
-      <c r="I2" s="54" t="s">
+      <c r="I2" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="N2" s="55" t="s">
+      <c r="J2" s="57"/>
+      <c r="K2" s="57"/>
+      <c r="L2" s="57"/>
+      <c r="N2" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="O2" s="55"/>
-      <c r="P2" s="55"/>
-      <c r="Q2" s="55"/>
-      <c r="S2" s="56" t="s">
+      <c r="O2" s="58"/>
+      <c r="P2" s="58"/>
+      <c r="Q2" s="58"/>
+      <c r="S2" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="T2" s="56"/>
-      <c r="U2" s="56"/>
-      <c r="V2" s="56"/>
-      <c r="X2" s="47" t="s">
+      <c r="T2" s="59"/>
+      <c r="U2" s="59"/>
+      <c r="V2" s="59"/>
+      <c r="X2" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="Y2" s="47"/>
-      <c r="Z2" s="47"/>
-      <c r="AA2" s="47"/>
-      <c r="AC2" s="48" t="s">
+      <c r="Y2" s="50"/>
+      <c r="Z2" s="50"/>
+      <c r="AA2" s="50"/>
+      <c r="AC2" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="AD2" s="48"/>
-      <c r="AE2" s="48"/>
-      <c r="AF2" s="48"/>
+      <c r="AD2" s="51"/>
+      <c r="AE2" s="51"/>
+      <c r="AF2" s="51"/>
     </row>
     <row r="3" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
@@ -2670,24 +2670,24 @@
         <v>40</v>
       </c>
       <c r="C3" s="16"/>
-      <c r="D3" s="49" t="s">
+      <c r="D3" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="50"/>
-      <c r="F3" s="52">
-        <v>43697</v>
-      </c>
-      <c r="G3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="55">
+        <v>43699</v>
+      </c>
+      <c r="G3" s="56"/>
       <c r="H3" s="18"/>
     </row>
     <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="49" t="s">
+      <c r="D4" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="50"/>
+      <c r="E4" s="53"/>
       <c r="F4" s="35">
         <v>0</v>
       </c>
@@ -2776,236 +2776,236 @@
       <c r="A5" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="51"/>
-      <c r="C5" s="51"/>
-      <c r="D5" s="51"/>
-      <c r="E5" s="51"/>
-      <c r="F5" s="51"/>
-      <c r="G5" s="51"/>
-      <c r="H5" s="51"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="54"/>
+      <c r="G5" s="54"/>
+      <c r="H5" s="54"/>
       <c r="I5" s="41">
         <f ca="1">IFERROR(Inicio_del_proyecto+Incremento_de_desplazamiento,TODAY())</f>
-        <v>43697</v>
+        <v>43699</v>
       </c>
       <c r="J5" s="42">
         <f ca="1">I5+1</f>
-        <v>43698</v>
+        <v>43700</v>
       </c>
       <c r="K5" s="42">
         <f t="shared" ref="K5:AX5" ca="1" si="0">J5+1</f>
-        <v>43699</v>
+        <v>43701</v>
       </c>
       <c r="L5" s="42">
         <f t="shared" ca="1" si="0"/>
-        <v>43700</v>
+        <v>43702</v>
       </c>
       <c r="M5" s="42">
         <f t="shared" ca="1" si="0"/>
-        <v>43701</v>
+        <v>43703</v>
       </c>
       <c r="N5" s="42">
         <f t="shared" ca="1" si="0"/>
-        <v>43702</v>
+        <v>43704</v>
       </c>
       <c r="O5" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>43703</v>
+        <v>43705</v>
       </c>
       <c r="P5" s="41">
         <f ca="1">O5+1</f>
-        <v>43704</v>
+        <v>43706</v>
       </c>
       <c r="Q5" s="42">
         <f ca="1">P5+1</f>
-        <v>43705</v>
+        <v>43707</v>
       </c>
       <c r="R5" s="42">
         <f t="shared" ca="1" si="0"/>
-        <v>43706</v>
+        <v>43708</v>
       </c>
       <c r="S5" s="42">
         <f t="shared" ca="1" si="0"/>
-        <v>43707</v>
+        <v>43709</v>
       </c>
       <c r="T5" s="42">
         <f t="shared" ca="1" si="0"/>
-        <v>43708</v>
+        <v>43710</v>
       </c>
       <c r="U5" s="42">
         <f t="shared" ca="1" si="0"/>
-        <v>43709</v>
+        <v>43711</v>
       </c>
       <c r="V5" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>43710</v>
+        <v>43712</v>
       </c>
       <c r="W5" s="41">
         <f ca="1">V5+1</f>
-        <v>43711</v>
+        <v>43713</v>
       </c>
       <c r="X5" s="42">
         <f ca="1">W5+1</f>
-        <v>43712</v>
+        <v>43714</v>
       </c>
       <c r="Y5" s="42">
         <f t="shared" ca="1" si="0"/>
-        <v>43713</v>
+        <v>43715</v>
       </c>
       <c r="Z5" s="42">
         <f t="shared" ca="1" si="0"/>
-        <v>43714</v>
+        <v>43716</v>
       </c>
       <c r="AA5" s="42">
         <f t="shared" ca="1" si="0"/>
-        <v>43715</v>
+        <v>43717</v>
       </c>
       <c r="AB5" s="42">
         <f t="shared" ca="1" si="0"/>
-        <v>43716</v>
+        <v>43718</v>
       </c>
       <c r="AC5" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>43717</v>
+        <v>43719</v>
       </c>
       <c r="AD5" s="41">
         <f ca="1">AC5+1</f>
-        <v>43718</v>
+        <v>43720</v>
       </c>
       <c r="AE5" s="42">
         <f ca="1">AD5+1</f>
-        <v>43719</v>
+        <v>43721</v>
       </c>
       <c r="AF5" s="42">
         <f t="shared" ca="1" si="0"/>
-        <v>43720</v>
+        <v>43722</v>
       </c>
       <c r="AG5" s="42">
         <f t="shared" ca="1" si="0"/>
-        <v>43721</v>
+        <v>43723</v>
       </c>
       <c r="AH5" s="42">
         <f t="shared" ca="1" si="0"/>
-        <v>43722</v>
+        <v>43724</v>
       </c>
       <c r="AI5" s="42">
         <f t="shared" ca="1" si="0"/>
-        <v>43723</v>
+        <v>43725</v>
       </c>
       <c r="AJ5" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>43724</v>
+        <v>43726</v>
       </c>
       <c r="AK5" s="41">
         <f ca="1">AJ5+1</f>
-        <v>43725</v>
+        <v>43727</v>
       </c>
       <c r="AL5" s="42">
         <f ca="1">AK5+1</f>
-        <v>43726</v>
+        <v>43728</v>
       </c>
       <c r="AM5" s="42">
         <f t="shared" ca="1" si="0"/>
-        <v>43727</v>
+        <v>43729</v>
       </c>
       <c r="AN5" s="42">
         <f t="shared" ca="1" si="0"/>
-        <v>43728</v>
+        <v>43730</v>
       </c>
       <c r="AO5" s="42">
         <f t="shared" ca="1" si="0"/>
-        <v>43729</v>
+        <v>43731</v>
       </c>
       <c r="AP5" s="42">
         <f t="shared" ca="1" si="0"/>
-        <v>43730</v>
+        <v>43732</v>
       </c>
       <c r="AQ5" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>43731</v>
+        <v>43733</v>
       </c>
       <c r="AR5" s="41">
         <f ca="1">AQ5+1</f>
-        <v>43732</v>
+        <v>43734</v>
       </c>
       <c r="AS5" s="42">
         <f ca="1">AR5+1</f>
-        <v>43733</v>
+        <v>43735</v>
       </c>
       <c r="AT5" s="42">
         <f t="shared" ca="1" si="0"/>
-        <v>43734</v>
+        <v>43736</v>
       </c>
       <c r="AU5" s="42">
         <f t="shared" ca="1" si="0"/>
-        <v>43735</v>
+        <v>43737</v>
       </c>
       <c r="AV5" s="42">
         <f t="shared" ca="1" si="0"/>
-        <v>43736</v>
+        <v>43738</v>
       </c>
       <c r="AW5" s="42">
         <f t="shared" ca="1" si="0"/>
-        <v>43737</v>
+        <v>43739</v>
       </c>
       <c r="AX5" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>43738</v>
+        <v>43740</v>
       </c>
       <c r="AY5" s="41">
         <f ca="1">AX5+1</f>
-        <v>43739</v>
+        <v>43741</v>
       </c>
       <c r="AZ5" s="42">
         <f ca="1">AY5+1</f>
-        <v>43740</v>
+        <v>43742</v>
       </c>
       <c r="BA5" s="42">
         <f t="shared" ref="BA5:BE5" ca="1" si="1">AZ5+1</f>
-        <v>43741</v>
+        <v>43743</v>
       </c>
       <c r="BB5" s="42">
         <f t="shared" ca="1" si="1"/>
-        <v>43742</v>
+        <v>43744</v>
       </c>
       <c r="BC5" s="42">
         <f t="shared" ca="1" si="1"/>
-        <v>43743</v>
+        <v>43745</v>
       </c>
       <c r="BD5" s="42">
         <f t="shared" ca="1" si="1"/>
-        <v>43744</v>
+        <v>43746</v>
       </c>
       <c r="BE5" s="43">
         <f t="shared" ca="1" si="1"/>
-        <v>43745</v>
+        <v>43747</v>
       </c>
       <c r="BF5" s="41">
         <f ca="1">BE5+1</f>
-        <v>43746</v>
+        <v>43748</v>
       </c>
       <c r="BG5" s="42">
         <f ca="1">BF5+1</f>
-        <v>43747</v>
+        <v>43749</v>
       </c>
       <c r="BH5" s="42">
         <f t="shared" ref="BH5:BL5" ca="1" si="2">BG5+1</f>
-        <v>43748</v>
+        <v>43750</v>
       </c>
       <c r="BI5" s="42">
         <f t="shared" ca="1" si="2"/>
-        <v>43749</v>
+        <v>43751</v>
       </c>
       <c r="BJ5" s="42">
         <f t="shared" ca="1" si="2"/>
-        <v>43750</v>
+        <v>43752</v>
       </c>
       <c r="BK5" s="42">
         <f t="shared" ca="1" si="2"/>
-        <v>43751</v>
+        <v>43753</v>
       </c>
       <c r="BL5" s="43">
         <f t="shared" ca="1" si="2"/>
-        <v>43752</v>
+        <v>43754</v>
       </c>
     </row>
     <row r="6" spans="1:64" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3095,227 +3095,227 @@
       <c r="H7" s="46"/>
       <c r="I7" s="21" t="str">
         <f t="shared" ref="I7" ca="1" si="3">LEFT(TEXT(I5,"ddd"),1)</f>
-        <v>m</v>
+        <v>j</v>
       </c>
       <c r="J7" s="21" t="str">
         <f t="shared" ref="J7:AR7" ca="1" si="4">LEFT(TEXT(J5,"ddd"),1)</f>
-        <v>m</v>
+        <v>v</v>
       </c>
       <c r="K7" s="21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>j</v>
+        <v>s</v>
       </c>
       <c r="L7" s="21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>v</v>
+        <v>d</v>
       </c>
       <c r="M7" s="21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>s</v>
+        <v>l</v>
       </c>
       <c r="N7" s="21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>d</v>
+        <v>m</v>
       </c>
       <c r="O7" s="21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>l</v>
+        <v>m</v>
       </c>
       <c r="P7" s="21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>m</v>
+        <v>j</v>
       </c>
       <c r="Q7" s="21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>m</v>
+        <v>v</v>
       </c>
       <c r="R7" s="21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>j</v>
+        <v>s</v>
       </c>
       <c r="S7" s="21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>v</v>
+        <v>d</v>
       </c>
       <c r="T7" s="21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>s</v>
+        <v>l</v>
       </c>
       <c r="U7" s="21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>d</v>
+        <v>m</v>
       </c>
       <c r="V7" s="21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>l</v>
+        <v>m</v>
       </c>
       <c r="W7" s="21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>m</v>
+        <v>j</v>
       </c>
       <c r="X7" s="21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>m</v>
+        <v>v</v>
       </c>
       <c r="Y7" s="21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>j</v>
+        <v>s</v>
       </c>
       <c r="Z7" s="21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>v</v>
+        <v>d</v>
       </c>
       <c r="AA7" s="21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>s</v>
+        <v>l</v>
       </c>
       <c r="AB7" s="21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>d</v>
+        <v>m</v>
       </c>
       <c r="AC7" s="21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>l</v>
+        <v>m</v>
       </c>
       <c r="AD7" s="21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>m</v>
+        <v>j</v>
       </c>
       <c r="AE7" s="21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>m</v>
+        <v>v</v>
       </c>
       <c r="AF7" s="21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>j</v>
+        <v>s</v>
       </c>
       <c r="AG7" s="21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>v</v>
+        <v>d</v>
       </c>
       <c r="AH7" s="21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>s</v>
+        <v>l</v>
       </c>
       <c r="AI7" s="21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>d</v>
+        <v>m</v>
       </c>
       <c r="AJ7" s="21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>l</v>
+        <v>m</v>
       </c>
       <c r="AK7" s="21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>m</v>
+        <v>j</v>
       </c>
       <c r="AL7" s="21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>m</v>
+        <v>v</v>
       </c>
       <c r="AM7" s="21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>j</v>
+        <v>s</v>
       </c>
       <c r="AN7" s="21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>v</v>
+        <v>d</v>
       </c>
       <c r="AO7" s="21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>s</v>
+        <v>l</v>
       </c>
       <c r="AP7" s="21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>d</v>
+        <v>m</v>
       </c>
       <c r="AQ7" s="21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>l</v>
+        <v>m</v>
       </c>
       <c r="AR7" s="21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>m</v>
+        <v>j</v>
       </c>
       <c r="AS7" s="21" t="str">
         <f t="shared" ref="AS7:BL7" ca="1" si="5">LEFT(TEXT(AS5,"ddd"),1)</f>
-        <v>m</v>
+        <v>v</v>
       </c>
       <c r="AT7" s="21" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>j</v>
+        <v>s</v>
       </c>
       <c r="AU7" s="21" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>v</v>
+        <v>d</v>
       </c>
       <c r="AV7" s="21" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>s</v>
+        <v>l</v>
       </c>
       <c r="AW7" s="21" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>d</v>
+        <v>m</v>
       </c>
       <c r="AX7" s="21" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>l</v>
+        <v>m</v>
       </c>
       <c r="AY7" s="21" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>m</v>
+        <v>j</v>
       </c>
       <c r="AZ7" s="21" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>m</v>
+        <v>v</v>
       </c>
       <c r="BA7" s="21" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>j</v>
+        <v>s</v>
       </c>
       <c r="BB7" s="21" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>v</v>
+        <v>d</v>
       </c>
       <c r="BC7" s="21" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>s</v>
+        <v>l</v>
       </c>
       <c r="BD7" s="21" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>d</v>
+        <v>m</v>
       </c>
       <c r="BE7" s="21" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>l</v>
+        <v>m</v>
       </c>
       <c r="BF7" s="21" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>m</v>
+        <v>j</v>
       </c>
       <c r="BG7" s="21" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>m</v>
+        <v>v</v>
       </c>
       <c r="BH7" s="21" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>j</v>
+        <v>s</v>
       </c>
       <c r="BI7" s="21" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>v</v>
+        <v>d</v>
       </c>
       <c r="BJ7" s="21" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>s</v>
+        <v>l</v>
       </c>
       <c r="BK7" s="21" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>d</v>
+        <v>m</v>
       </c>
       <c r="BL7" s="21" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>l</v>
+        <v>m</v>
       </c>
     </row>
     <row r="8" spans="1:64" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -3625,7 +3625,7 @@
     </row>
     <row r="10" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
-      <c r="B10" s="58" t="s">
+      <c r="B10" s="48" t="s">
         <v>39</v>
       </c>
       <c r="C10" s="28" t="s">
@@ -3633,22 +3633,22 @@
       </c>
       <c r="D10" s="28"/>
       <c r="E10" s="25">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
       <c r="F10" s="26">
         <v>43699</v>
       </c>
       <c r="G10" s="27">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H10" s="22"/>
-      <c r="I10" s="31" t="str">
+      <c r="I10" s="31">
         <f ca="1">IF(AND($C10="Objetivo",I$5&gt;=$F10,I$5&lt;=$F10+$G10-1),2,IF(AND($C10="Hito",I$5&gt;=$F10,I$5&lt;=$F10+$G10-1),1,""))</f>
-        <v/>
-      </c>
-      <c r="J10" s="31" t="str">
+        <v>1</v>
+      </c>
+      <c r="J10" s="31">
         <f t="shared" ca="1" si="6"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="K10" s="31">
         <f t="shared" ca="1" si="6"/>
@@ -3658,9 +3658,9 @@
         <f t="shared" ca="1" si="6"/>
         <v>1</v>
       </c>
-      <c r="M10" s="31" t="str">
+      <c r="M10" s="31">
         <f t="shared" ca="1" si="6"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="N10" s="31" t="str">
         <f t="shared" ca="1" si="6"/>
@@ -3869,7 +3869,7 @@
     </row>
     <row r="11" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
-      <c r="B11" s="57" t="s">
+      <c r="B11" s="47" t="s">
         <v>35</v>
       </c>
       <c r="C11" s="28" t="s">
@@ -3880,10 +3880,10 @@
         <v>1</v>
       </c>
       <c r="F11" s="26">
-        <v>43699</v>
+        <v>43705</v>
       </c>
       <c r="G11" s="27">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H11" s="22"/>
       <c r="I11" s="31" t="str">
@@ -4113,7 +4113,7 @@
     </row>
     <row r="12" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
-      <c r="B12" s="57" t="s">
+      <c r="B12" s="47" t="s">
         <v>36</v>
       </c>
       <c r="C12" s="28" t="s">
@@ -4121,13 +4121,13 @@
       </c>
       <c r="D12" s="28"/>
       <c r="E12" s="25">
-        <v>0.8</v>
+        <v>0.2</v>
       </c>
       <c r="F12" s="26">
-        <v>43699</v>
+        <v>43682</v>
       </c>
       <c r="G12" s="27">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H12" s="22"/>
       <c r="I12" s="31" t="str">
@@ -4138,13 +4138,13 @@
         <f t="shared" ca="1" si="6"/>
         <v/>
       </c>
-      <c r="K12" s="31">
+      <c r="K12" s="31" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="L12" s="31">
+        <v/>
+      </c>
+      <c r="L12" s="31" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>2</v>
+        <v/>
       </c>
       <c r="M12" s="31" t="str">
         <f t="shared" ca="1" si="6"/>
@@ -4357,7 +4357,7 @@
     </row>
     <row r="13" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
-      <c r="B13" s="57" t="s">
+      <c r="B13" s="47" t="s">
         <v>37</v>
       </c>
       <c r="C13" s="28" t="s">
@@ -4365,13 +4365,13 @@
       </c>
       <c r="D13" s="28"/>
       <c r="E13" s="25">
-        <v>0.8</v>
+        <v>0.2</v>
       </c>
       <c r="F13" s="26">
-        <v>43699</v>
+        <v>43713</v>
       </c>
       <c r="G13" s="27">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H13" s="22"/>
       <c r="I13" s="31" t="str">
@@ -4382,73 +4382,73 @@
         <f t="shared" ca="1" si="6"/>
         <v/>
       </c>
-      <c r="K13" s="31">
+      <c r="K13" s="31" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v/>
+      </c>
+      <c r="L13" s="31" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v/>
+      </c>
+      <c r="M13" s="31" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v/>
+      </c>
+      <c r="N13" s="31" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v/>
+      </c>
+      <c r="O13" s="31" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v/>
+      </c>
+      <c r="P13" s="31" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v/>
+      </c>
+      <c r="Q13" s="31" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v/>
+      </c>
+      <c r="R13" s="31" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v/>
+      </c>
+      <c r="S13" s="31" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v/>
+      </c>
+      <c r="T13" s="31" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v/>
+      </c>
+      <c r="U13" s="31" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v/>
+      </c>
+      <c r="V13" s="31" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v/>
+      </c>
+      <c r="W13" s="31">
         <f t="shared" ca="1" si="6"/>
         <v>2</v>
       </c>
-      <c r="L13" s="31">
+      <c r="X13" s="31">
         <f t="shared" ca="1" si="6"/>
         <v>2</v>
       </c>
-      <c r="M13" s="31" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="N13" s="31" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="O13" s="31" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="P13" s="31" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="Q13" s="31" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="R13" s="31" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="S13" s="31" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="T13" s="31" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="U13" s="31" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="V13" s="31" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="W13" s="31" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="X13" s="31" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="Y13" s="31" t="str">
+      <c r="Y13" s="31">
         <f t="shared" ca="1" si="7"/>
-        <v/>
-      </c>
-      <c r="Z13" s="31" t="str">
+        <v>2</v>
+      </c>
+      <c r="Z13" s="31">
         <f t="shared" ca="1" si="7"/>
-        <v/>
-      </c>
-      <c r="AA13" s="31" t="str">
+        <v>2</v>
+      </c>
+      <c r="AA13" s="31">
         <f t="shared" ca="1" si="7"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="AB13" s="31" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -4601,7 +4601,7 @@
     </row>
     <row r="14" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
-      <c r="B14" s="57" t="s">
+      <c r="B14" s="47" t="s">
         <v>38</v>
       </c>
       <c r="C14" s="28" t="s">
@@ -4612,10 +4612,10 @@
         <v>0</v>
       </c>
       <c r="F14" s="26">
-        <v>43699</v>
+        <v>43717</v>
       </c>
       <c r="G14" s="27">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H14" s="22"/>
       <c r="I14" s="31" t="str">
@@ -4626,13 +4626,13 @@
         <f t="shared" ca="1" si="6"/>
         <v/>
       </c>
-      <c r="K14" s="31">
+      <c r="K14" s="31" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="L14" s="31">
+        <v/>
+      </c>
+      <c r="L14" s="31" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>2</v>
+        <v/>
       </c>
       <c r="M14" s="31" t="str">
         <f t="shared" ca="1" si="6"/>
@@ -4690,25 +4690,25 @@
         <f t="shared" ca="1" si="7"/>
         <v/>
       </c>
-      <c r="AA14" s="31" t="str">
+      <c r="AA14" s="31">
         <f t="shared" ca="1" si="7"/>
-        <v/>
-      </c>
-      <c r="AB14" s="31" t="str">
+        <v>2</v>
+      </c>
+      <c r="AB14" s="31">
         <f t="shared" ca="1" si="7"/>
-        <v/>
-      </c>
-      <c r="AC14" s="31" t="str">
+        <v>2</v>
+      </c>
+      <c r="AC14" s="31">
         <f t="shared" ca="1" si="7"/>
-        <v/>
-      </c>
-      <c r="AD14" s="31" t="str">
+        <v>2</v>
+      </c>
+      <c r="AD14" s="31">
         <f t="shared" ca="1" si="7"/>
-        <v/>
-      </c>
-      <c r="AE14" s="31" t="str">
+        <v>2</v>
+      </c>
+      <c r="AE14" s="31">
         <f t="shared" ca="1" si="7"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="AF14" s="31" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -4845,7 +4845,7 @@
     </row>
     <row r="15" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13"/>
-      <c r="B15" s="57"/>
+      <c r="B15" s="47"/>
       <c r="C15" s="28"/>
       <c r="D15" s="28"/>
       <c r="E15" s="25"/>
@@ -5079,7 +5079,7 @@
     </row>
     <row r="16" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="13"/>
-      <c r="B16" s="59"/>
+      <c r="B16" s="49"/>
       <c r="C16" s="28"/>
       <c r="D16" s="28"/>
       <c r="E16" s="25"/>
@@ -5287,7 +5287,7 @@
         <v/>
       </c>
       <c r="BG16" s="31" t="str">
-        <f t="shared" ref="BG16:BP20" ca="1" si="18">IF(AND($C15="Objetivo",BG$5&gt;=$F15,BG$5&lt;=$F15+$G15-1),2,IF(AND($C15="Hito",BG$5&gt;=$F15,BG$5&lt;=$F15+$G15-1),1,""))</f>
+        <f t="shared" ref="BG16:BL20" ca="1" si="18">IF(AND($C15="Objetivo",BG$5&gt;=$F15,BG$5&lt;=$F15+$G15-1),2,IF(AND($C15="Hito",BG$5&gt;=$F15,BG$5&lt;=$F15+$G15-1),1,""))</f>
         <v/>
       </c>
       <c r="BH16" s="31" t="str">
@@ -5313,7 +5313,7 @@
     </row>
     <row r="17" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12"/>
-      <c r="B17" s="59"/>
+      <c r="B17" s="49"/>
       <c r="C17" s="28"/>
       <c r="D17" s="28"/>
       <c r="E17" s="25"/>
@@ -9437,141 +9437,141 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5:BL34">
-    <cfRule type="expression" dxfId="38" priority="1">
+    <cfRule type="expression" dxfId="41" priority="1">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:AM4">
-    <cfRule type="expression" dxfId="37" priority="7">
+    <cfRule type="expression" dxfId="40" priority="7">
       <formula>I$5&lt;=EOMONTH($I$5,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:BL4">
-    <cfRule type="expression" dxfId="36" priority="3">
+    <cfRule type="expression" dxfId="39" priority="3">
       <formula>AND(J$5&lt;=EOMONTH($I$5,2),J$5&gt;EOMONTH($I$5,0),J$5&gt;EOMONTH($I$5,1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:BL4">
-    <cfRule type="expression" dxfId="35" priority="2">
+    <cfRule type="expression" dxfId="38" priority="2">
       <formula>AND(I$5&lt;=EOMONTH($I$5,1),I$5&gt;EOMONTH($I$5,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8:BL14">
-    <cfRule type="expression" dxfId="34" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="24" stopIfTrue="1">
       <formula>AND($C8="Riesgo bajo",I$5&gt;=$F8,I$5&lt;=$F8+$G8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="43" stopIfTrue="1">
       <formula>AND($C8="Riesgo alto",I$5&gt;=$F8,I$5&lt;=$F8+$G8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="61" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="61" stopIfTrue="1">
       <formula>AND($C8="Según lo previsto",I$5&gt;=$F8,I$5&lt;=$F8+$G8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="62" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="62" stopIfTrue="1">
       <formula>AND($C8="Riesgo medio",I$5&gt;=$F8,I$5&lt;=$F8+$G8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="63" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="63" stopIfTrue="1">
       <formula>AND(LEN($C8)=0,I$5&gt;=$F8,I$5&lt;=$F8+$G8-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16:BL20">
-    <cfRule type="expression" dxfId="29" priority="90" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="90" stopIfTrue="1">
       <formula>AND($C15="Riesgo bajo",I$5&gt;=$F15,I$5&lt;=$F15+$G15-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="91" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="91" stopIfTrue="1">
       <formula>AND($C15="Riesgo alto",I$5&gt;=$F15,I$5&lt;=$F15+$G15-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="92" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="92" stopIfTrue="1">
       <formula>AND($C15="Según lo previsto",I$5&gt;=$F15,I$5&lt;=$F15+$G15-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="93" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="93" stopIfTrue="1">
       <formula>AND($C15="Riesgo medio",I$5&gt;=$F15,I$5&lt;=$F15+$G15-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="94" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="94" stopIfTrue="1">
       <formula>AND(LEN($C15)=0,I$5&gt;=$F15,I$5&lt;=$F15+$G15-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I22:BL26">
-    <cfRule type="expression" dxfId="24" priority="114" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="114" stopIfTrue="1">
       <formula>AND($C20="Riesgo bajo",I$5&gt;=$F20,I$5&lt;=$F20+$G20-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="115" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="115" stopIfTrue="1">
       <formula>AND($C20="Riesgo alto",I$5&gt;=$F20,I$5&lt;=$F20+$G20-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="116" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="116" stopIfTrue="1">
       <formula>AND($C20="Según lo previsto",I$5&gt;=$F20,I$5&lt;=$F20+$G20-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="117" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="117" stopIfTrue="1">
       <formula>AND($C20="Riesgo medio",I$5&gt;=$F20,I$5&lt;=$F20+$G20-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="118" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="118" stopIfTrue="1">
       <formula>AND(LEN($C20)=0,I$5&gt;=$F20,I$5&lt;=$F20+$G20-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I28:BL33">
-    <cfRule type="expression" dxfId="19" priority="143" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="143" stopIfTrue="1">
       <formula>AND($C25="Riesgo bajo",I$5&gt;=$F25,I$5&lt;=$F25+$G25-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="144" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="144" stopIfTrue="1">
       <formula>AND($C25="Riesgo alto",I$5&gt;=$F25,I$5&lt;=$F25+$G25-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="145" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="145" stopIfTrue="1">
       <formula>AND($C25="Según lo previsto",I$5&gt;=$F25,I$5&lt;=$F25+$G25-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="146" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="146" stopIfTrue="1">
       <formula>AND($C25="Riesgo medio",I$5&gt;=$F25,I$5&lt;=$F25+$G25-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="147" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="147" stopIfTrue="1">
       <formula>AND(LEN($C25)=0,I$5&gt;=$F25,I$5&lt;=$F25+$G25-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I27:BL27">
-    <cfRule type="expression" dxfId="14" priority="150" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="150" stopIfTrue="1">
       <formula>AND($C36="Riesgo bajo",I$5&gt;=$F36,I$5&lt;=$F36+$G36-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="151" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="151" stopIfTrue="1">
       <formula>AND($C36="Riesgo alto",I$5&gt;=$F36,I$5&lt;=$F36+$G36-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="152" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="152" stopIfTrue="1">
       <formula>AND($C36="Según lo previsto",I$5&gt;=$F36,I$5&lt;=$F36+$G36-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="153" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="153" stopIfTrue="1">
       <formula>AND($C36="Riesgo medio",I$5&gt;=$F36,I$5&lt;=$F36+$G36-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="154" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="154" stopIfTrue="1">
       <formula>AND(LEN($C36)=0,I$5&gt;=$F36,I$5&lt;=$F36+$G36-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I21:BL21">
-    <cfRule type="expression" dxfId="9" priority="155" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="155" stopIfTrue="1">
       <formula>AND($C35="Riesgo bajo",I$5&gt;=$F35,I$5&lt;=$F35+$G35-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="156" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="156" stopIfTrue="1">
       <formula>AND($C35="Riesgo alto",I$5&gt;=$F35,I$5&lt;=$F35+$G35-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="157" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="157" stopIfTrue="1">
       <formula>AND($C35="Según lo previsto",I$5&gt;=$F35,I$5&lt;=$F35+$G35-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="158" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="158" stopIfTrue="1">
       <formula>AND($C35="Riesgo medio",I$5&gt;=$F35,I$5&lt;=$F35+$G35-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="159" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="159" stopIfTrue="1">
       <formula>AND(LEN($C35)=0,I$5&gt;=$F35,I$5&lt;=$F35+$G35-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I15:BL15">
-    <cfRule type="expression" dxfId="4" priority="160" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="160" stopIfTrue="1">
       <formula>AND($C34="Riesgo bajo",I$5&gt;=$F34,I$5&lt;=$F34+$G34-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="161" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="161" stopIfTrue="1">
       <formula>AND($C34="Riesgo alto",I$5&gt;=$F34,I$5&lt;=$F34+$G34-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="162" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="162" stopIfTrue="1">
       <formula>AND($C34="Según lo previsto",I$5&gt;=$F34,I$5&lt;=$F34+$G34-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="163" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="163" stopIfTrue="1">
       <formula>AND($C34="Riesgo medio",I$5&gt;=$F34,I$5&lt;=$F34+$G34-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="164" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="164" stopIfTrue="1">
       <formula>AND(LEN($C34)=0,I$5&gt;=$F34,I$5&lt;=$F34+$G34-1)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Agregue el txt BD
Se colocaron los itegrantes del equipo BD

Co-Authored-By: David Velázquez <steinervalue@users.noreply.github.com>
Co-Authored-By: ismaelmargarito <ismaelmargarito@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Cronograma y tiempo/Cronograma BD.xlsx
+++ b/Cronograma y tiempo/Cronograma BD.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{305835F7-1252-49D9-A270-40BF02AB6CFD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{350DD35F-0757-4A22-B5E4-752243D9FEF9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
   <si>
     <t>Cree un diagrama de Gantt en esta hoja de cálculo.
 Escriba el título de este proyecto en la celda B1. 
@@ -186,17 +186,20 @@
   <si>
     <t>Equipo de Base de datos</t>
   </si>
+  <si>
+    <t>Agregar tabla de cookies</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="5">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="d"/>
-    <numFmt numFmtId="168" formatCode="#,##0_ ;\-#,##0\ "/>
+    <numFmt numFmtId="166" formatCode="d"/>
+    <numFmt numFmtId="167" formatCode="#,##0_ ;\-#,##0\ "/>
   </numFmts>
   <fonts count="28" x14ac:knownFonts="1">
     <font>
@@ -880,7 +883,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="1" applyFont="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="1" applyFont="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyProtection="0">
@@ -892,7 +895,7 @@
     <xf numFmtId="14" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1001,7 +1004,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="9" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="10" applyFont="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="10" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1039,13 +1042,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="13" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="13" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="13" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="13" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="13" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="13" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1094,55 +1097,55 @@
     </xf>
   </cellXfs>
   <cellStyles count="50">
-    <cellStyle name="20% - Énfasis1" xfId="27" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis2" xfId="31" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis3" xfId="35" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis4" xfId="39" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis5" xfId="43" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis6" xfId="47" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis1" xfId="28" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis2" xfId="32" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis3" xfId="36" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis4" xfId="40" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis5" xfId="44" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis6" xfId="48" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis1" xfId="29" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis2" xfId="33" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis3" xfId="37" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis4" xfId="41" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis5" xfId="45" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis6" xfId="49" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Bueno" xfId="14" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Cálculo" xfId="19" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Celda de comprobación" xfId="21" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Celda vinculada" xfId="20" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Encabezado 1" xfId="6" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Encabezado 4" xfId="13" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Énfasis1" xfId="26" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Énfasis2" xfId="30" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Énfasis3" xfId="34" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Énfasis4" xfId="38" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Énfasis5" xfId="42" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Énfasis6" xfId="46" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Entrada" xfId="17" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="27" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="31" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="35" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="39" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="43" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="47" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="28" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="32" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="36" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="40" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="48" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="29" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="33" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="37" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="41" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="49" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="26" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="30" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="34" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="38" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="42" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="15" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="19" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="21" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Comma" xfId="4" builtinId="3" customBuiltin="1"/>
+    <cellStyle name="Comma [0]" xfId="10" builtinId="6" customBuiltin="1"/>
+    <cellStyle name="Currency" xfId="11" builtinId="4" customBuiltin="1"/>
+    <cellStyle name="Currency [0]" xfId="12" builtinId="7" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="24" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Fecha" xfId="9" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8" customBuiltin="1"/>
-    <cellStyle name="Incorrecto" xfId="15" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Millares" xfId="4" builtinId="3" customBuiltin="1"/>
-    <cellStyle name="Millares [0]" xfId="10" builtinId="6" customBuiltin="1"/>
-    <cellStyle name="Moneda" xfId="11" builtinId="4" customBuiltin="1"/>
-    <cellStyle name="Moneda [0]" xfId="12" builtinId="7" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="14" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="6" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="7" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="8" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="13" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="17" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="16" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Notas" xfId="23" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Porcentaje" xfId="2" builtinId="5" customBuiltin="1"/>
-    <cellStyle name="Salida" xfId="18" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Texto de advertencia" xfId="22" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Texto explicativo" xfId="24" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Título" xfId="5" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Título 2" xfId="7" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Título 3" xfId="8" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="23" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="18" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="5" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="25" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="22" builtinId="11" customBuiltin="1"/>
     <cellStyle name="zHiddenText" xfId="3" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
   </cellStyles>
   <dxfs count="54">
@@ -2587,11 +2590,11 @@
   </sheetPr>
   <dimension ref="A1:BL40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.7109375" style="12" customWidth="1"/>
     <col min="2" max="2" width="67.28515625" bestFit="1" customWidth="1"/>
@@ -2693,7 +2696,7 @@
       </c>
       <c r="I4" s="34" t="str">
         <f ca="1">TEXT(I5,"mmmm")</f>
-        <v>agosto</v>
+        <v>August</v>
       </c>
       <c r="J4" s="34"/>
       <c r="K4" s="34"/>
@@ -2713,7 +2716,7 @@
       <c r="V4" s="34"/>
       <c r="W4" s="34" t="str">
         <f ca="1">IF(OR(TEXT(W5,"mmmm")=P4,TEXT(W5,"mmmm")=I4),"",TEXT(W5,"mmmm"))</f>
-        <v>septiembre</v>
+        <v>September</v>
       </c>
       <c r="X4" s="34"/>
       <c r="Y4" s="34"/>
@@ -2753,7 +2756,7 @@
       <c r="AX4" s="34"/>
       <c r="AY4" s="34" t="str">
         <f ca="1">IF(OR(TEXT(AY5,"mmmm")=AR4,TEXT(AY5,"mmmm")=AK4,TEXT(AY5,"mmmm")=AD4,TEXT(AY5,"mmmm")=W4),"",TEXT(AY5,"mmmm"))</f>
-        <v>octubre</v>
+        <v>October</v>
       </c>
       <c r="AZ4" s="34"/>
       <c r="BA4" s="34"/>
@@ -3095,227 +3098,227 @@
       <c r="H7" s="46"/>
       <c r="I7" s="21" t="str">
         <f t="shared" ref="I7" ca="1" si="3">LEFT(TEXT(I5,"ddd"),1)</f>
-        <v>j</v>
+        <v>T</v>
       </c>
       <c r="J7" s="21" t="str">
         <f t="shared" ref="J7:AR7" ca="1" si="4">LEFT(TEXT(J5,"ddd"),1)</f>
-        <v>v</v>
+        <v>F</v>
       </c>
       <c r="K7" s="21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>s</v>
+        <v>S</v>
       </c>
       <c r="L7" s="21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>d</v>
+        <v>S</v>
       </c>
       <c r="M7" s="21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>l</v>
+        <v>M</v>
       </c>
       <c r="N7" s="21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>m</v>
+        <v>T</v>
       </c>
       <c r="O7" s="21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>m</v>
+        <v>W</v>
       </c>
       <c r="P7" s="21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>j</v>
+        <v>T</v>
       </c>
       <c r="Q7" s="21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>v</v>
+        <v>F</v>
       </c>
       <c r="R7" s="21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>s</v>
+        <v>S</v>
       </c>
       <c r="S7" s="21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>d</v>
+        <v>S</v>
       </c>
       <c r="T7" s="21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>l</v>
+        <v>M</v>
       </c>
       <c r="U7" s="21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>m</v>
+        <v>T</v>
       </c>
       <c r="V7" s="21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>m</v>
+        <v>W</v>
       </c>
       <c r="W7" s="21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>j</v>
+        <v>T</v>
       </c>
       <c r="X7" s="21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>v</v>
+        <v>F</v>
       </c>
       <c r="Y7" s="21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>s</v>
+        <v>S</v>
       </c>
       <c r="Z7" s="21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>d</v>
+        <v>S</v>
       </c>
       <c r="AA7" s="21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>l</v>
+        <v>M</v>
       </c>
       <c r="AB7" s="21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>m</v>
+        <v>T</v>
       </c>
       <c r="AC7" s="21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>m</v>
+        <v>W</v>
       </c>
       <c r="AD7" s="21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>j</v>
+        <v>T</v>
       </c>
       <c r="AE7" s="21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>v</v>
+        <v>F</v>
       </c>
       <c r="AF7" s="21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>s</v>
+        <v>S</v>
       </c>
       <c r="AG7" s="21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>d</v>
+        <v>S</v>
       </c>
       <c r="AH7" s="21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>l</v>
+        <v>M</v>
       </c>
       <c r="AI7" s="21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>m</v>
+        <v>T</v>
       </c>
       <c r="AJ7" s="21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>m</v>
+        <v>W</v>
       </c>
       <c r="AK7" s="21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>j</v>
+        <v>T</v>
       </c>
       <c r="AL7" s="21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>v</v>
+        <v>F</v>
       </c>
       <c r="AM7" s="21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>s</v>
+        <v>S</v>
       </c>
       <c r="AN7" s="21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>d</v>
+        <v>S</v>
       </c>
       <c r="AO7" s="21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>l</v>
+        <v>M</v>
       </c>
       <c r="AP7" s="21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>m</v>
+        <v>T</v>
       </c>
       <c r="AQ7" s="21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>m</v>
+        <v>W</v>
       </c>
       <c r="AR7" s="21" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>j</v>
+        <v>T</v>
       </c>
       <c r="AS7" s="21" t="str">
         <f t="shared" ref="AS7:BL7" ca="1" si="5">LEFT(TEXT(AS5,"ddd"),1)</f>
-        <v>v</v>
+        <v>F</v>
       </c>
       <c r="AT7" s="21" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>s</v>
+        <v>S</v>
       </c>
       <c r="AU7" s="21" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>d</v>
+        <v>S</v>
       </c>
       <c r="AV7" s="21" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>l</v>
+        <v>M</v>
       </c>
       <c r="AW7" s="21" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>m</v>
+        <v>T</v>
       </c>
       <c r="AX7" s="21" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>m</v>
+        <v>W</v>
       </c>
       <c r="AY7" s="21" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>j</v>
+        <v>T</v>
       </c>
       <c r="AZ7" s="21" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>v</v>
+        <v>F</v>
       </c>
       <c r="BA7" s="21" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>s</v>
+        <v>S</v>
       </c>
       <c r="BB7" s="21" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>d</v>
+        <v>S</v>
       </c>
       <c r="BC7" s="21" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>l</v>
+        <v>M</v>
       </c>
       <c r="BD7" s="21" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>m</v>
+        <v>T</v>
       </c>
       <c r="BE7" s="21" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>m</v>
+        <v>W</v>
       </c>
       <c r="BF7" s="21" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>j</v>
+        <v>T</v>
       </c>
       <c r="BG7" s="21" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>v</v>
+        <v>F</v>
       </c>
       <c r="BH7" s="21" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>s</v>
+        <v>S</v>
       </c>
       <c r="BI7" s="21" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>d</v>
+        <v>S</v>
       </c>
       <c r="BJ7" s="21" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>l</v>
+        <v>M</v>
       </c>
       <c r="BK7" s="21" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>m</v>
+        <v>T</v>
       </c>
       <c r="BL7" s="21" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>m</v>
+        <v>W</v>
       </c>
     </row>
     <row r="8" spans="1:64" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -4845,12 +4848,22 @@
     </row>
     <row r="15" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13"/>
-      <c r="B15" s="47"/>
-      <c r="C15" s="28"/>
+      <c r="B15" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="28" t="s">
+        <v>15</v>
+      </c>
       <c r="D15" s="28"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="27"/>
+      <c r="E15" s="25">
+        <v>0</v>
+      </c>
+      <c r="F15" s="26">
+        <v>43718</v>
+      </c>
+      <c r="G15" s="27">
+        <v>3</v>
+      </c>
       <c r="H15" s="22"/>
       <c r="I15" s="31" t="str">
         <f t="shared" ref="I15:AN15" ca="1" si="11">IF(AND($C34="Objetivo",I$5&gt;=$F34,I$5&lt;=$F34+$G34-1),2,IF(AND($C34="Hito",I$5&gt;=$F34,I$5&lt;=$F34+$G34-1),1,""))</f>
@@ -5162,17 +5175,17 @@
         <f t="shared" ca="1" si="14"/>
         <v/>
       </c>
-      <c r="AB16" s="31" t="str">
+      <c r="AB16" s="31">
         <f t="shared" ca="1" si="14"/>
-        <v/>
-      </c>
-      <c r="AC16" s="31" t="str">
+        <v>2</v>
+      </c>
+      <c r="AC16" s="31">
         <f t="shared" ref="AC16:AL20" ca="1" si="15">IF(AND($C15="Objetivo",AC$5&gt;=$F15,AC$5&lt;=$F15+$G15-1),2,IF(AND($C15="Hito",AC$5&gt;=$F15,AC$5&lt;=$F15+$G15-1),1,""))</f>
-        <v/>
-      </c>
-      <c r="AD16" s="31" t="str">
+        <v>2</v>
+      </c>
+      <c r="AD16" s="31">
         <f t="shared" ca="1" si="15"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="AE16" s="31" t="str">
         <f t="shared" ca="1" si="15"/>
@@ -9692,7 +9705,7 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="87.140625" style="8" customWidth="1"/>
     <col min="2" max="16384" width="9.140625" style="6"/>

</xml_diff>